<commit_message>
Invoice generation exl template added and invoice pdf generated successfully.
</commit_message>
<xml_diff>
--- a/Assets/Template/TemplateInvoice.xlsx
+++ b/Assets/Template/TemplateInvoice.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="61">
   <si>
     <t>SHIVANI DHOOP INDUSTRIES</t>
   </si>
@@ -116,97 +117,103 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>Amount Chargeable (in words)</t>
+  </si>
+  <si>
+    <t>E. &amp; O.E</t>
+  </si>
+  <si>
+    <t>Total Tax Amount</t>
+  </si>
+  <si>
+    <t>SGST/UTGST</t>
+  </si>
+  <si>
+    <t>CGST</t>
+  </si>
+  <si>
+    <t>Taxable Value</t>
+  </si>
+  <si>
+    <t>Tax Amount (in words):</t>
+  </si>
+  <si>
+    <t>Company's Bank Details</t>
+  </si>
+  <si>
+    <t>A/c Holder's Name:</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Branch &amp; IFS Code:</t>
+  </si>
+  <si>
+    <t>SWIFT Code:</t>
+  </si>
+  <si>
+    <t>A/c No.:</t>
+  </si>
+  <si>
+    <t>Authorised Signatory</t>
+  </si>
+  <si>
+    <t>Company's PAN:</t>
+  </si>
+  <si>
+    <t>Declaration</t>
+  </si>
+  <si>
+    <t>We declare that this invoice shows the actual price of the goods described and that all particulars are true and correct.</t>
+  </si>
+  <si>
+    <t>This is a Computer Generated Invoice</t>
+  </si>
+  <si>
+    <t>Tax Invoice</t>
+  </si>
+  <si>
+    <t>{{StateName &amp; Code}}</t>
+  </si>
+  <si>
+    <t>{{PhoneNo}}</t>
+  </si>
+  <si>
+    <t>{{EmailID}}</t>
+  </si>
+  <si>
+    <t>{{GSTNo}}</t>
+  </si>
+  <si>
+    <t>{{Full Add}}</t>
+  </si>
+  <si>
+    <t>Disc.%</t>
+  </si>
+  <si>
+    <t>{{Amount in words}}</t>
+  </si>
+  <si>
+    <t>{{Tax Details}}</t>
+  </si>
+  <si>
+    <t>{{Address}}</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Amount Chargeable (in words)</t>
-  </si>
-  <si>
-    <t>E. &amp; O.E</t>
-  </si>
-  <si>
-    <t>INR One Lakh Ninety Six Thousand One Hundred Seventy Six Only</t>
-  </si>
-  <si>
-    <t>Total Tax Amount</t>
-  </si>
-  <si>
-    <t>SGST/UTGST</t>
-  </si>
-  <si>
-    <t>CGST</t>
-  </si>
-  <si>
-    <t>Taxable Value</t>
-  </si>
-  <si>
-    <t>Tax Amount (in words):</t>
-  </si>
-  <si>
-    <t>INR Nine Thousand Nine Hundred Thirty Six Only</t>
-  </si>
-  <si>
-    <t>Company's Bank Details</t>
-  </si>
-  <si>
-    <t>A/c Holder's Name:</t>
-  </si>
-  <si>
-    <t>Bank Name</t>
-  </si>
-  <si>
-    <t>Branch &amp; IFS Code:</t>
-  </si>
-  <si>
-    <t>SWIFT Code:</t>
-  </si>
-  <si>
-    <t>A/c No.:</t>
-  </si>
-  <si>
-    <t>Authorised Signatory</t>
-  </si>
-  <si>
-    <t>Company's PAN:</t>
-  </si>
-  <si>
-    <t>Declaration</t>
-  </si>
-  <si>
-    <t>We declare that this invoice shows the actual price of the goods described and that all particulars are true and correct.</t>
-  </si>
-  <si>
-    <t>This is a Computer Generated Invoice</t>
-  </si>
-  <si>
-    <t>Tax Invoice</t>
-  </si>
-  <si>
-    <t>{{StateName &amp; Code}}</t>
-  </si>
-  <si>
-    <t>{{PhoneNo}}</t>
-  </si>
-  <si>
-    <t>{{EmailID}}</t>
-  </si>
-  <si>
-    <t>{{GSTNo}}</t>
-  </si>
-  <si>
-    <t>{{Full Add}}</t>
-  </si>
-  <si>
-    <t>Disc.%</t>
+    <t>IGST</t>
+  </si>
+  <si>
+    <t>{{Tax amt in words}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;₹&quot;\ #,##0.00;[Red]&quot;₹&quot;\ \-#,##0.00"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -436,11 +443,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -529,29 +549,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -567,6 +624,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -576,12 +639,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -652,10 +709,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -693,12 +750,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -708,44 +798,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,6 +857,55 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="371475" y="647701"/>
+          <a:ext cx="1002526" cy="1009649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>257176</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>592951</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1079,10 +1203,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1090,7 +1214,7 @@
     <col min="1" max="1" width="5.42578125" style="30" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" style="30" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
@@ -1102,34 +1226,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="A1" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="70"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="75" t="s">
+      <c r="A2" s="81"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="76"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1138,9 +1262,9 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1157,19 +1281,19 @@
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="65"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1178,19 +1302,19 @@
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="65"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1199,21 +1323,21 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="65"/>
+      <c r="E6" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1222,16 +1346,16 @@
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="55"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1245,20 +1369,20 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
+      <c r="E8" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1268,16 +1392,16 @@
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="55"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1291,23 +1415,23 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="47" t="s">
+      <c r="H10" s="60"/>
+      <c r="I10" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="49"/>
-      <c r="K10" s="48"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1316,19 +1440,19 @@
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="46"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1337,19 +1461,19 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="78"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="47" t="s">
+      <c r="A12" s="89"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="56"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1358,17 +1482,19 @@
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="46"/>
+      <c r="A13" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1377,23 +1503,23 @@
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="47" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="47" t="s">
+      <c r="H14" s="59"/>
+      <c r="I14" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="49"/>
-      <c r="K14" s="48"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1406,15 +1532,15 @@
         <v>9</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="46"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1427,19 +1553,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="47" t="s">
+      <c r="G16" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="48"/>
-      <c r="I16" s="47" t="s">
+      <c r="H16" s="59"/>
+      <c r="I16" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="48"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="59"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1452,15 +1578,15 @@
         <v>4</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="46"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="57"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1469,23 +1595,23 @@
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="48"/>
-      <c r="I18" s="47" t="s">
+      <c r="H18" s="59"/>
+      <c r="I18" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="48"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="59"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1494,19 +1620,19 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="84"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="95"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1515,21 +1641,21 @@
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="47" t="s">
+      <c r="A20" s="89"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="47" t="s">
+      <c r="H20" s="59"/>
+      <c r="I20" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="48"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1538,17 +1664,19 @@
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="46"/>
+      <c r="A21" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="57"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1557,23 +1685,23 @@
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="47" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="47" t="s">
+      <c r="H22" s="59"/>
+      <c r="I22" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="49"/>
-      <c r="K22" s="48"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="59"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1586,15 +1714,15 @@
         <v>9</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="46"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="57"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1607,17 +1735,17 @@
         <v>3</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="48"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="59"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1630,15 +1758,15 @@
         <v>4</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="88"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="99"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1653,11 +1781,11 @@
       <c r="D26" s="16"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="89"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="91"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="102"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1669,12 +1797,12 @@
       <c r="A27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="18" t="s">
         <v>14</v>
       </c>
@@ -1688,7 +1816,7 @@
         <v>16</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>29</v>
@@ -1702,10 +1830,10 @@
     </row>
     <row r="28" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
       <c r="F28" s="25"/>
       <c r="G28" s="26"/>
       <c r="H28" s="27"/>
@@ -1721,10 +1849,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="24"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="52"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
       <c r="F29" s="25"/>
       <c r="G29" s="26"/>
       <c r="H29" s="31"/>
@@ -1740,10 +1868,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="24"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="52"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
       <c r="F30" s="25"/>
       <c r="G30" s="26"/>
       <c r="H30" s="31"/>
@@ -1759,10 +1887,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="24"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="52"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="65"/>
       <c r="F31" s="25"/>
       <c r="G31" s="26"/>
       <c r="H31" s="31"/>
@@ -1778,10 +1906,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="24"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="65"/>
       <c r="F32" s="25"/>
       <c r="G32" s="26"/>
       <c r="H32" s="31"/>
@@ -1797,10 +1925,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="24"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="65"/>
       <c r="F33" s="25"/>
       <c r="G33" s="26"/>
       <c r="H33" s="31"/>
@@ -1816,10 +1944,10 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="24"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="52"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
       <c r="F34" s="25"/>
       <c r="G34" s="26"/>
       <c r="H34" s="31"/>
@@ -1835,10 +1963,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="24"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
       <c r="F35" s="25"/>
       <c r="G35" s="26"/>
       <c r="H35" s="31"/>
@@ -1854,10 +1982,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="24"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="52"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="65"/>
       <c r="F36" s="25"/>
       <c r="G36" s="26"/>
       <c r="H36" s="31"/>
@@ -1873,10 +2001,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="24"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="52"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
       <c r="F37" s="25"/>
       <c r="G37" s="26"/>
       <c r="H37" s="31"/>
@@ -1892,10 +2020,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="24"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="52"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="25"/>
       <c r="G38" s="26"/>
       <c r="H38" s="31"/>
@@ -1911,10 +2039,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="24"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="52"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
       <c r="F39" s="25"/>
       <c r="G39" s="26"/>
       <c r="H39" s="31"/>
@@ -1930,10 +2058,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="24"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="65"/>
       <c r="F40" s="25"/>
       <c r="G40" s="26"/>
       <c r="H40" s="31"/>
@@ -1949,10 +2077,10 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="24"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="52"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
       <c r="F41" s="25"/>
       <c r="G41" s="26"/>
       <c r="H41" s="31"/>
@@ -1968,10 +2096,10 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="24"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="52"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="65"/>
       <c r="F42" s="25"/>
       <c r="G42" s="26"/>
       <c r="H42" s="31"/>
@@ -1987,10 +2115,10 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="24"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="52"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="65"/>
       <c r="F43" s="25"/>
       <c r="G43" s="26"/>
       <c r="H43" s="31"/>
@@ -2005,17 +2133,19 @@
       <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="33"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="104" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="104"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="39"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -2024,404 +2154,312 @@
       <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
+      <c r="A45" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="109"/>
+      <c r="C45" s="109"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="34" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="33"/>
+      <c r="A46" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="117"/>
+      <c r="C46" s="117"/>
+      <c r="D46" s="117"/>
+      <c r="E46" s="117"/>
+      <c r="F46" s="117"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="117"/>
+      <c r="I46" s="117"/>
+      <c r="J46" s="117"/>
+      <c r="K46" s="118"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="24"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="33"/>
+      <c r="A47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="103"/>
+      <c r="E47" s="93" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="113" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="113"/>
+      <c r="H47" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="113"/>
+      <c r="J47" s="113"/>
+      <c r="K47" s="112" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="33"/>
+      <c r="A48" s="103"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="113"/>
+      <c r="K48" s="112"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="37"/>
+      <c r="A49" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="106"/>
+      <c r="C49" s="106"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="114"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="39"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="92" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="93"/>
-      <c r="C50" s="93"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="A50" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="109"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="110" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="110"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="110"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="111"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" s="95"/>
-      <c r="C51" s="95"/>
-      <c r="D51" s="95"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="95"/>
-      <c r="G51" s="95"/>
-      <c r="H51" s="95"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="96"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="5"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="100" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="100"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="82" t="s">
+      <c r="A52" s="24"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="107" t="s">
-        <v>36</v>
-      </c>
-      <c r="G52" s="107"/>
-      <c r="H52" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="I52" s="107"/>
-      <c r="J52" s="107"/>
-      <c r="K52" s="106" t="s">
-        <v>34</v>
-      </c>
+      <c r="G52" s="64"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="5"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="100"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="100"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="H53" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="J53" s="107"/>
-      <c r="K53" s="106"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="80"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="67"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="101"/>
-      <c r="B54" s="102"/>
-      <c r="C54" s="102"/>
-      <c r="D54" s="103"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="108"/>
-      <c r="J54" s="109"/>
-      <c r="K54" s="35"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54" s="64"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="67"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="98"/>
-      <c r="C55" s="98"/>
-      <c r="D55" s="99"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="108"/>
-      <c r="J55" s="109"/>
-      <c r="K55" s="35"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="67"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="93"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="E56" s="104"/>
-      <c r="F56" s="104"/>
-      <c r="G56" s="104"/>
-      <c r="H56" s="104"/>
-      <c r="I56" s="104"/>
-      <c r="J56" s="104"/>
-      <c r="K56" s="105"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G56" s="55"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="67"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="5"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="67"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="29"/>
+      <c r="A58" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="73"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="G58" s="51"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="5"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
+      <c r="J58" s="68"/>
+      <c r="K58" s="69"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="24"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="G59" s="69"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="44"/>
-      <c r="J59" s="44"/>
-      <c r="K59" s="56"/>
+      <c r="A59" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="5"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G60" s="51"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="44"/>
-      <c r="K60" s="56"/>
+      <c r="A60" s="74"/>
+      <c r="B60" s="75"/>
+      <c r="C60" s="75"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="5"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="56"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="44" t="s">
+      <c r="A61" s="77"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="78"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="79"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="G62" s="44"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="44"/>
-      <c r="J62" s="44"/>
-      <c r="K62" s="56"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="50" t="s">
+      <c r="K61" s="71"/>
+    </row>
+    <row r="62" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="55"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="56"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="62"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="41"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="58"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65" s="64"/>
-      <c r="C65" s="64"/>
-      <c r="D65" s="64"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="5"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="63"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="65"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="5"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="66"/>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="K67" s="60"/>
-    </row>
-    <row r="68" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="53"/>
-      <c r="G68" s="53"/>
-      <c r="H68" s="53"/>
-      <c r="I68" s="53"/>
-      <c r="J68" s="53"/>
-      <c r="K68" s="53"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I55:J55"/>
+  <mergeCells count="101">
+    <mergeCell ref="A49:D49"/>
     <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:K46"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A52:D53"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="A47:D48"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:E32"/>
@@ -2444,7 +2482,6 @@
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="A22:B22"/>
@@ -2457,8 +2494,7 @@
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:F20"/>
     <mergeCell ref="C22:F22"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="H56:K56"/>
     <mergeCell ref="A2:C9"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="E7:F7"/>
@@ -2481,34 +2517,1380 @@
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A62:K62"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B36:E36"/>
-    <mergeCell ref="H63:K63"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:E67"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H59:K59"/>
-    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:E61"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="H55:K55"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="84" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="81"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="82"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="55"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="55"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="60"/>
+      <c r="I10" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="60"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="89"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="59"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="59"/>
+      <c r="I14" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="60"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="59"/>
+      <c r="I16" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="60"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="59"/>
+      <c r="I18" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="60"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="89"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="59"/>
+      <c r="I20" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="60"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="59"/>
+      <c r="I22" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="60"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+    </row>
+    <row r="28" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="24"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="24"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="24"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="24"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="24"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="24"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="24"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="24"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="24"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="47"/>
+      <c r="B44" s="104" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="104"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="109"/>
+      <c r="C45" s="109"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="117"/>
+      <c r="C46" s="117"/>
+      <c r="D46" s="117"/>
+      <c r="E46" s="117"/>
+      <c r="F46" s="117"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="117"/>
+      <c r="I46" s="117"/>
+      <c r="J46" s="117"/>
+      <c r="K46" s="118"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="122"/>
+      <c r="C47" s="122"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="113" t="s">
+        <v>59</v>
+      </c>
+      <c r="I47" s="113"/>
+      <c r="J47" s="113"/>
+      <c r="K47" s="112" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="124"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="125"/>
+      <c r="F48" s="126"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="113"/>
+      <c r="K48" s="112"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="106"/>
+      <c r="C49" s="106"/>
+      <c r="D49" s="106"/>
+      <c r="E49" s="106"/>
+      <c r="F49" s="107"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="114"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="48"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="109"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="110" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="110"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="110"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="111"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="24"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="24"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="64"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="24"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="80"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="67"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54" s="64"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="67"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="24"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="67"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="24"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G56" s="55"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="67"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="67"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="73"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
+      <c r="J58" s="68"/>
+      <c r="K58" s="69"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="74"/>
+      <c r="B60" s="75"/>
+      <c r="C60" s="75"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="77"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="78"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="79"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K61" s="71"/>
+    </row>
+    <row r="62" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="100">
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="A59:E61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="A62:K62"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="A47:F48"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="G25:K26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A19:F20"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="A11:F12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:C9"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="84" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>